<commit_message>
updated Wireless LED workshop component specification
</commit_message>
<xml_diff>
--- a/Workshop costs.xlsx
+++ b/Workshop costs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/c_m_v_riet_student_tue_nl/Documents/Studie/#MSc2/Soldering workshops/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/c_m_v_riet_student_tue_nl/Documents/DESIGN/Github/Soldering Workshops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="481" documentId="13_ncr:1_{ABAB46C6-B7E1-4C0B-AA70-CE2A569E2D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F13E98C-87FB-433A-AAC5-0E427E5F00F4}"/>
+  <xr:revisionPtr revIDLastSave="492" documentId="13_ncr:1_{ABAB46C6-B7E1-4C0B-AA70-CE2A569E2D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A414CFFB-3321-420E-8D4E-310A50D8298A}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="2340" windowWidth="21600" windowHeight="11505" firstSheet="1" activeTab="5" xr2:uid="{37414339-373C-4A92-8C15-0502F53297DB}"/>
+    <workbookView xWindow="1290" yWindow="1890" windowWidth="21600" windowHeight="11505" firstSheet="1" activeTab="1" xr2:uid="{37414339-373C-4A92-8C15-0502F53297DB}"/>
   </bookViews>
   <sheets>
     <sheet name="overview balance" sheetId="6" r:id="rId1"/>
@@ -53,15 +53,9 @@
     <t>total</t>
   </si>
   <si>
-    <t>LMC555xN</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
-    <t>https://nl.rs-online.com/web/p/op-amps/1977336/</t>
-  </si>
-  <si>
     <t>TC4426</t>
   </si>
   <si>
@@ -366,6 +360,12 @@
   </si>
   <si>
     <t>alleen 1 ATTiny type op voorraad</t>
+  </si>
+  <si>
+    <t>TLC555CP</t>
+  </si>
+  <si>
+    <t>https://nl.rs-online.com/web/p/timer-circuits/1977574</t>
   </si>
 </sst>
 </file>
@@ -774,37 +774,37 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="7">
         <f>'Wireless LEDs'!D25</f>
-        <v>5.0612166666666667</v>
+        <v>4.437216666666667</v>
       </c>
       <c r="C2" s="7">
         <v>5</v>
       </c>
       <c r="D2" s="7">
         <f>C2-B2</f>
-        <v>-6.1216666666666697E-2</v>
+        <v>0.56278333333333297</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="7">
         <f>Lighthouse!D11</f>
@@ -820,7 +820,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="7">
         <f>Moduli!D15</f>
@@ -836,7 +836,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="7">
         <f>Cube!D25</f>
@@ -852,7 +852,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="7">
         <f>Lotus!D21</f>
@@ -872,7 +872,7 @@
       </c>
       <c r="B8" s="8">
         <f>SUM(B2:B6)</f>
-        <v>20.901121324492468</v>
+        <v>20.27712132449247</v>
       </c>
       <c r="C8" s="8">
         <f>SUM(C2:C6)</f>
@@ -880,7 +880,7 @@
       </c>
       <c r="D8" s="8">
         <f>SUM(D2:D6)</f>
-        <v>4.0988786755075317</v>
+        <v>4.7228786755075314</v>
       </c>
     </row>
   </sheetData>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1988EF83-736F-424F-BA8F-20008381E626}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J16:J17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,13 +925,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -945,17 +945,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="C3" s="4">
-        <v>1.68</v>
+        <v>1.056</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:D7" si="0">A3*C3</f>
-        <v>1.68</v>
+        <v>1.056</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
@@ -965,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4">
         <v>1.4</v>
@@ -975,7 +975,7 @@
         <v>1.4</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
@@ -985,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4">
         <v>7.1999999999999995E-2</v>
@@ -995,7 +995,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="2"/>
@@ -1007,7 +1007,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4">
         <v>0.09</v>
@@ -1017,10 +1017,10 @@
         <v>0.18</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="M6" s="3"/>
       <c r="R6" s="4"/>
@@ -1031,7 +1031,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4">
         <v>0.05</v>
@@ -1041,7 +1041,7 @@
         <v>0.05</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4">
         <v>6.4000000000000001E-2</v>
@@ -1061,7 +1061,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
@@ -1071,7 +1071,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="4">
         <v>3.1E-2</v>
@@ -1081,7 +1081,7 @@
         <v>0.217</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
@@ -1091,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4">
         <v>2.1000000000000001E-2</v>
@@ -1101,7 +1101,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="2"/>
@@ -1113,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="4">
         <v>7.3999999999999996E-2</v>
@@ -1123,7 +1123,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
@@ -1133,7 +1133,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="4">
         <v>0.17599999999999999</v>
@@ -1142,8 +1142,8 @@
         <f t="shared" si="1"/>
         <v>0.17599999999999999</v>
       </c>
-      <c r="F12" t="s">
-        <v>32</v>
+      <c r="F12" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -1153,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4">
         <v>0.185</v>
@@ -1163,7 +1163,7 @@
         <v>0.185</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
@@ -1174,13 +1174,13 @@
       </c>
       <c r="D14" s="5">
         <f>SUM(D3:D13)</f>
-        <v>4.1189999999999998</v>
+        <v>3.4950000000000001</v>
       </c>
       <c r="S14" s="5"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D16" s="4"/>
       <c r="S16" s="4"/>
@@ -1190,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2">
         <f>20.78/30</f>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="2">
         <f>6.47/400</f>
@@ -1231,7 +1231,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2">
         <f>(2.47+1.52)/50</f>
@@ -1249,7 +1249,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2">
         <f>2.88/100</f>
@@ -1274,19 +1274,19 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D25" s="5">
         <f>SUM(D14:D22)</f>
-        <v>5.0612166666666667</v>
+        <v>4.437216666666667</v>
       </c>
       <c r="S25" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{900AC433-81C3-431B-904D-9E354130039E}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{83275B4F-0DB9-459C-B671-3C767EA85AF6}"/>
-    <hyperlink ref="F13" r:id="rId3" xr:uid="{DDAC75B6-4259-41ED-881B-410EBA19079C}"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{83275B4F-0DB9-459C-B671-3C767EA85AF6}"/>
+    <hyperlink ref="F13" r:id="rId2" xr:uid="{DDAC75B6-4259-41ED-881B-410EBA19079C}"/>
+    <hyperlink ref="F12" r:id="rId3" xr:uid="{EF704E66-8A63-4BF2-AF0C-A2B619133A0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
@@ -1310,7 +1310,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1329,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1343,7 +1343,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4">
         <f>4.16/100</f>
@@ -1354,7 +1354,7 @@
         <v>8.3199999999999996E-2</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1362,7 +1362,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="4">
         <v>4.2999999999999997E-2</v>
@@ -1372,7 +1372,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1380,7 +1380,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4">
         <v>3.1E-2</v>
@@ -1390,7 +1390,7 @@
         <v>0.124</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1398,7 +1398,7 @@
         <v>1.2</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="4">
         <f>11.91/50.9</f>
@@ -1409,7 +1409,7 @@
         <v>0.28078585461689587</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1417,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4">
         <f>2.15/100</f>
@@ -1428,7 +1428,7 @@
         <v>2.1499999999999998E-2</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C9" s="4">
         <f>3.15/8</f>
@@ -1447,12 +1447,12 @@
         <v>0.39374999999999999</v>
       </c>
       <c r="F9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" s="5">
         <f>SUM(D4:D9)</f>
@@ -1519,7 +1519,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1538,13 +1538,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="4">
         <v>2.1999999999999999E-2</v>
@@ -1562,7 +1562,7 @@
         <v>0.21999999999999997</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1570,7 +1570,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" s="4">
         <f>2.08/100</f>
@@ -1581,7 +1581,7 @@
         <v>0.20799999999999999</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1589,7 +1589,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="4">
         <f>6.23/100</f>
@@ -1600,7 +1600,7 @@
         <v>6.2300000000000001E-2</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1608,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" s="4">
         <f>6.54/30</f>
@@ -1619,7 +1619,7 @@
         <v>0.218</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4">
         <f>3.18/50</f>
@@ -1638,7 +1638,7 @@
         <v>6.3600000000000004E-2</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
         <v>1.5</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="4">
         <f>11.91/50.9</f>
@@ -1657,7 +1657,7 @@
         <v>0.35098231827111981</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1671,7 +1671,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" s="4"/>
     </row>
@@ -1680,7 +1680,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2">
         <f>13.33/100</f>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" s="4">
         <f>D13+D10</f>
@@ -1742,7 +1742,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1761,13 +1761,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1775,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4">
         <f>6.54/30</f>
@@ -1786,7 +1786,7 @@
         <v>0.218</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1794,7 +1794,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4">
         <v>0.313</v>
@@ -1804,7 +1804,7 @@
         <v>0.313</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1812,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6" s="4">
         <v>1.1499999999999999</v>
@@ -1822,7 +1822,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1830,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4">
         <v>0.16500000000000001</v>
@@ -1840,7 +1840,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1848,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="4">
         <v>0.22500000000000001</v>
@@ -1858,7 +1858,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1866,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" s="4">
         <v>0.16300000000000001</v>
@@ -1876,7 +1876,7 @@
         <v>0.16300000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="4">
         <v>3.4000000000000002E-2</v>
@@ -1894,7 +1894,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1902,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="4">
         <v>0.17100000000000001</v>
@@ -1912,7 +1912,7 @@
         <v>0.17100000000000001</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1920,7 +1920,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="4">
         <v>3.1E-2</v>
@@ -1930,7 +1930,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1938,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C13" s="4">
         <v>0.10299999999999999</v>
@@ -1948,7 +1948,7 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="F13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1956,7 +1956,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C14" s="10">
         <f>5.47/20</f>
@@ -1968,7 +1968,7 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1976,7 +1976,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C15" s="10">
         <f>5.29/20</f>
@@ -1987,7 +1987,7 @@
         <v>0.79350000000000009</v>
       </c>
       <c r="F15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1995,7 +1995,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C16" s="10">
         <f>5.29/20</f>
@@ -2006,7 +2006,7 @@
         <v>0.79350000000000009</v>
       </c>
       <c r="F16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C17" s="10">
         <f>5.29/20</f>
@@ -2025,7 +2025,7 @@
         <v>0.79350000000000009</v>
       </c>
       <c r="F17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2033,7 +2033,7 @@
         <v>0.5</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" s="4">
         <f>11.91/50.9</f>
@@ -2044,7 +2044,7 @@
         <v>0.11699410609037328</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2052,7 +2052,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C19" s="4">
         <f>2.25/2/400</f>
@@ -2063,12 +2063,12 @@
         <v>8.4375000000000006E-3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D20" s="5">
         <f>SUM(D4:D19)</f>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D22" s="4"/>
     </row>
@@ -2086,7 +2086,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C23" s="2">
         <f>3.1/5</f>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D25" s="5">
         <f>D23+D20</f>
@@ -2125,7 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED23811-4CDF-469E-8091-506DBC73F0E4}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -2138,7 +2138,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -2157,13 +2157,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2171,7 +2171,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4">
         <v>0.154</v>
@@ -2181,7 +2181,7 @@
         <v>0.46199999999999997</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2189,7 +2189,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4">
         <v>3.1E-2</v>
@@ -2199,7 +2199,7 @@
         <v>0.58899999999999997</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -2207,7 +2207,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C6" s="4">
         <v>2.5600000000000001E-2</v>
@@ -2217,7 +2217,7 @@
         <v>0.38400000000000001</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4">
         <v>0.2</v>
@@ -2235,7 +2235,7 @@
         <v>0.2</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2243,7 +2243,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4">
         <f>2.94/100</f>
@@ -2254,7 +2254,7 @@
         <v>2.9399999999999999E-2</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="4">
         <v>2.5</v>
@@ -2272,10 +2272,10 @@
         <v>2.5</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" t="s">
         <v>51</v>
-      </c>
-      <c r="P9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2283,7 +2283,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="4">
         <v>0.123</v>
@@ -2293,7 +2293,7 @@
         <v>0.123</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2301,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4">
         <v>0.154</v>
@@ -2311,7 +2311,7 @@
         <v>0.154</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2319,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="4">
         <v>0.16500000000000001</v>
@@ -2329,7 +2329,7 @@
         <v>0.16500000000000001</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2337,7 +2337,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="4">
         <f>6.23/100</f>
@@ -2348,7 +2348,7 @@
         <v>6.2300000000000001E-2</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2356,7 +2356,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4">
         <f>6.54/30</f>
@@ -2367,7 +2367,7 @@
         <v>0.218</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2375,7 +2375,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="4">
         <f>11.91/50.9</f>
@@ -2386,7 +2386,7 @@
         <v>0.23398821218074656</v>
       </c>
       <c r="F15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18" s="4"/>
     </row>
@@ -2412,7 +2412,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2">
         <f>20.78/30</f>
@@ -2423,12 +2423,12 @@
         <v>0.69266666666666665</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D21" s="5">
         <f>D19+D16</f>
@@ -2445,16 +2445,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G25" s="4">
         <v>1.024</v>

</xml_diff>

<commit_message>
Added Controller workshop to costs
</commit_message>
<xml_diff>
--- a/Workshop costs.xlsx
+++ b/Workshop costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/c_m_v_riet_student_tue_nl/Documents/DESIGN/Github/Soldering Workshops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="587" documentId="13_ncr:1_{ABAB46C6-B7E1-4C0B-AA70-CE2A569E2D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A948704-40F7-4EE3-92E2-2DBCB613E859}"/>
+  <xr:revisionPtr revIDLastSave="736" documentId="13_ncr:1_{ABAB46C6-B7E1-4C0B-AA70-CE2A569E2D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{401E1BB4-59E5-43C8-9C4D-FEF14A5B6991}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{37414339-373C-4A92-8C15-0502F53297DB}"/>
+    <workbookView xWindow="10275" yWindow="1035" windowWidth="15420" windowHeight="13935" firstSheet="2" activeTab="6" xr2:uid="{37414339-373C-4A92-8C15-0502F53297DB}"/>
   </bookViews>
   <sheets>
     <sheet name="overview balance" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Moduli" sheetId="3" r:id="rId4"/>
     <sheet name="Cube" sheetId="4" r:id="rId5"/>
     <sheet name="Lotus" sheetId="5" r:id="rId6"/>
+    <sheet name="Controller" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="140">
   <si>
     <t>BOM</t>
   </si>
@@ -384,6 +385,81 @@
   </si>
   <si>
     <t>dip socket 8 pins</t>
+  </si>
+  <si>
+    <t>push button 6x6x5</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/shop/en/switches/manual-switches/pcb-switches/tactile-push-button-switch-momentary-4pin-6*6*5mm</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/shop/en/cables-and-connectors/cables-and-adapters/prototyping-wires/copper-wire/synflex-v-180-enameled-copper-wire-0.4mm-250g</t>
+  </si>
+  <si>
+    <t>enamelled wire</t>
+  </si>
+  <si>
+    <t>acrylic</t>
+  </si>
+  <si>
+    <t>https://www.kunststofshop.nl/acrylaat-plexiglas/acrylaat-platen/transparant-standaard-maten/acrylaat-plaat-transparant-500x500x3mm/a-3443-20000030</t>
+  </si>
+  <si>
+    <t>M3 bolt</t>
+  </si>
+  <si>
+    <t>header female</t>
+  </si>
+  <si>
+    <t>tie wrap</t>
+  </si>
+  <si>
+    <t>https://www.kingmicroschroeven.nl/bzk-inbus-verzonkenkopschroef-staal-din-7991-m3x16.html</t>
+  </si>
+  <si>
+    <t>M3 nut</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/shop/en/tools-and-mounting/installation-and-mounting-material/nuts/m3-nut-100-pieces</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/shop/en/cables-and-connectors/connectors/pin-headers/female/12-pins-header-female</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/shop/en/tools-and-mounting/installation-and-mounting-material/cable-ties-zip-ties-tyraps/perel-set-with-nylon-cable-ties-tyraps-75-pieces-black</t>
+  </si>
+  <si>
+    <t>foamboard</t>
+  </si>
+  <si>
+    <t>free from leftovers Expl Making?</t>
+  </si>
+  <si>
+    <t>shipping Tiny</t>
+  </si>
+  <si>
+    <t>shipping is €2.50 for envelope mail</t>
+  </si>
+  <si>
+    <t>Total per kit:</t>
+  </si>
+  <si>
+    <t>Ordering for 15 kits:</t>
+  </si>
+  <si>
+    <t>shipping is €5.95 for parcel</t>
+  </si>
+  <si>
+    <t>Total for 15 kits</t>
+  </si>
+  <si>
+    <t>Total per kit</t>
+  </si>
+  <si>
+    <t>printing PLA</t>
+  </si>
+  <si>
+    <t>printing</t>
   </si>
 </sst>
 </file>
@@ -911,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1988EF83-736F-424F-BA8F-20008381E626}">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,4 +2641,578 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399C0E57-CE64-4764-B25E-9B474CAAFF87}">
+  <dimension ref="A1:I42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="71.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D12" si="0">A3*C3</f>
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="4">
+        <f>9.92/223</f>
+        <v>4.4484304932735426E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>4.4484304932735426E-2</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="4">
+        <f>(13.25+8.95)*100/121/27</f>
+        <v>0.67952249770431594</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.67952249770431594</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="4">
+        <f>(8.84+2.99)*100/121/100</f>
+        <v>9.7768595041322306E-2</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.39107438016528923</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="4">
+        <f>2.48/100</f>
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>9.9199999999999997E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="4">
+        <f>1.45/75</f>
+        <v>1.9333333333333334E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>1.9333333333333334E-2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="4">
+        <f>5.95*100/121/14</f>
+        <v>0.3512396694214876</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.3512396694214876</v>
+      </c>
+      <c r="F11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5">
+        <f>SUM(D3:D12)</f>
+        <v>2.9448541855571615</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2">
+        <f>(19+14.85)/30</f>
+        <v>1.1283333333333334</v>
+      </c>
+      <c r="D17" s="4">
+        <f>C17/A17</f>
+        <v>1.1283333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="5">
+        <f>SUM(D14:D17)</f>
+        <v>4.0731875188904949</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="4">
+        <f>7.5*100/121</f>
+        <v>6.1983471074380168</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" ref="D25:D34" si="1">A25*C25</f>
+        <v>6.1983471074380168</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="4">
+        <v>9.92</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="1"/>
+        <v>9.92</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="4">
+        <f>(13.25+8.95)*100/121</f>
+        <v>18.347107438016529</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="1"/>
+        <v>18.347107438016529</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="4">
+        <f>(8.84+2.99)*100/121</f>
+        <v>9.776859504132231</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="1"/>
+        <v>9.776859504132231</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="4">
+        <f>2.48</f>
+        <v>2.48</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="1"/>
+        <v>2.48</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="4">
+        <v>6.94</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="1"/>
+        <v>6.94</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1.45</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="1"/>
+        <v>1.45</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="4">
+        <f>5.95*100/121</f>
+        <v>4.9173553719008263</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="1"/>
+        <v>4.9173553719008263</v>
+      </c>
+      <c r="F33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="4">
+        <f>0.3*15</f>
+        <v>4.5</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="5">
+        <f>SUM(D25:D33)</f>
+        <v>60.029669421487604</v>
+      </c>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="2">
+        <f>(11.5+11.41)</f>
+        <v>22.91</v>
+      </c>
+      <c r="D39" s="4">
+        <f>C39/A39</f>
+        <v>22.91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="5">
+        <f>SUM(D36:D39)</f>
+        <v>82.939669421487608</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" s="4">
+        <f>D41/15</f>
+        <v>5.5293112947658409</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{7E0BF3B6-2555-4708-9B57-4EB6488930B8}"/>
+    <hyperlink ref="F25" r:id="rId2" xr:uid="{C6855C31-EAA0-4D44-A21C-75B653E927C8}"/>
+    <hyperlink ref="F26" r:id="rId3" xr:uid="{7985B287-9202-49BA-96EC-3527E35AF464}"/>
+    <hyperlink ref="F29" r:id="rId4" xr:uid="{B904EA2C-A916-49E4-90BF-86FCFF073D72}"/>
+    <hyperlink ref="F30" r:id="rId5" xr:uid="{53E6BBBE-F583-4BE3-82C8-B8CA2353E487}"/>
+    <hyperlink ref="F31" r:id="rId6" xr:uid="{77B9EDD2-CF55-42EF-9CB8-820F71732DB2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Controller update and workshop cost update
</commit_message>
<xml_diff>
--- a/Workshop costs.xlsx
+++ b/Workshop costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - TU Eindhoven\DESIGN\Github\Soldering Workshops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAE32AC-E3FD-4531-B9A3-0CD86F168E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89375C9-745C-4FEF-BCB3-01DBF7715341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="75" windowWidth="18300" windowHeight="13995" firstSheet="1" activeTab="6" xr2:uid="{37414339-373C-4A92-8C15-0502F53297DB}"/>
+    <workbookView xWindow="29760" yWindow="2640" windowWidth="21600" windowHeight="11505" firstSheet="1" activeTab="6" xr2:uid="{37414339-373C-4A92-8C15-0502F53297DB}"/>
   </bookViews>
   <sheets>
     <sheet name="overview balance" sheetId="6" r:id="rId1"/>
@@ -2666,8 +2666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399C0E57-CE64-4764-B25E-9B474CAAFF87}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2967,12 +2967,12 @@
         <v>17</v>
       </c>
       <c r="C19" s="2">
-        <f>(19+14.85)/30</f>
-        <v>1.1283333333333334</v>
+        <f>(13.33+12.84)*100/121</f>
+        <v>21.628099173553718</v>
       </c>
       <c r="D19" s="4">
-        <f>C19/A19</f>
-        <v>1.1283333333333334</v>
+        <f>C19/20</f>
+        <v>1.0814049586776859</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2984,7 +2984,7 @@
       </c>
       <c r="D21" s="5">
         <f>SUM(D16:D19)</f>
-        <v>4.025849266244462</v>
+        <v>3.9789208915888139</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3267,18 +3267,18 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
         <v>17</v>
       </c>
       <c r="C43" s="2">
-        <f>31.1/20</f>
-        <v>1.5550000000000002</v>
+        <f>(13.33+12.84)*100/121</f>
+        <v>21.628099173553718</v>
       </c>
       <c r="D43" s="4">
-        <f>C43/A43</f>
-        <v>1.5550000000000002</v>
+        <f>C43</f>
+        <v>21.628099173553718</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -3290,7 +3290,7 @@
       </c>
       <c r="D45" s="5">
         <f>SUM(D40:D43)</f>
-        <v>60.607937537547286</v>
+        <v>80.681036711101001</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="D46" s="4">
         <f>D45/15</f>
-        <v>4.0405291691698189</v>
+        <v>5.3787357807400671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>